<commit_message>
added tests for constants class
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -620,16 +620,16 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>12.4</v>
+        <v>2.0</v>
       </c>
       <c r="B2" s="2">
-        <v>21.4</v>
+        <v>2.0</v>
       </c>
       <c r="C2" s="2">
-        <v>30.3</v>
+        <v>2.0</v>
       </c>
       <c r="D2" s="2">
-        <v>46.2</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix birth outcome names
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -5,16 +5,16 @@
   <sheets>
     <sheet state="visible" name="total mortality" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="mortality" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="RRStunting" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="RRWasting" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="RRBreastfeeding" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="distributions" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="birth distribution" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="time between births" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="RR birth by type" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="RR birth by time" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="OR stunting progression" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="distributions" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="RRStunting" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="RRWasting" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="birth distribution" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="time between births" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="RR birth by type" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="RR birth by time" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="OR birth outcome stunting" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="54">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -110,54 +110,54 @@
     <t>Other</t>
   </si>
   <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Stunting</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>mild</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>Wasting</t>
+  </si>
+  <si>
+    <t>Breastfeeding</t>
+  </si>
+  <si>
+    <t>exclusive</t>
+  </si>
+  <si>
+    <t>predominant</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
     <t>Stunting Status</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>mild</t>
-  </si>
-  <si>
-    <t>moderate</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
     <t>Wasting Status</t>
   </si>
   <si>
     <t>Breastfeeding Status</t>
   </si>
   <si>
-    <t>exclusive</t>
-  </si>
-  <si>
-    <t>predominant</t>
-  </si>
-  <si>
-    <t>partial</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>Distribution</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Stunting</t>
-  </si>
-  <si>
-    <t>Wasting</t>
-  </si>
-  <si>
-    <t>Breastfeeding</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -188,28 +188,19 @@
     <t>&lt;24 months</t>
   </si>
   <si>
-    <t>pretermSGA</t>
-  </si>
-  <si>
-    <t>pretermAGA</t>
-  </si>
-  <si>
-    <t>termSGA</t>
+    <t>Pre-term SGA</t>
+  </si>
+  <si>
+    <t>Pre-term AGA</t>
+  </si>
+  <si>
+    <t>Term SGA</t>
   </si>
   <si>
     <t>Outcome</t>
   </si>
   <si>
     <t>Term AGA</t>
-  </si>
-  <si>
-    <t>Term SGA</t>
-  </si>
-  <si>
-    <t>Pre-term AGA</t>
-  </si>
-  <si>
-    <t>Pre-term SGA</t>
   </si>
 </sst>
 </file>
@@ -383,156 +374,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
+      <c r="A2" s="2">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="2">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.0</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -552,66 +411,152 @@
         <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.0</v>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="2">
-        <v>3.03</v>
+        <v>3.14</v>
       </c>
       <c r="D2" s="2">
-        <v>1.77</v>
+        <v>1.73</v>
       </c>
       <c r="E2" s="2">
-        <v>1.0</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -628,31 +573,71 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
+      <c r="A1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>2.0</v>
+      <c r="A2" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B2" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="2">
-        <v>2.0</v>
+        <v>3.03</v>
       </c>
       <c r="D2" s="2">
-        <v>2.0</v>
+        <v>1.77</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.49</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -672,13 +657,13 @@
         <v>53</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -1081,10 +1066,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1103,11 +1088,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
+      <c r="A2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -1127,7 +1112,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
@@ -1147,7 +1132,7 @@
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -1167,7 +1152,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -1186,11 +1171,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>15</v>
+      <c r="A6" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
@@ -1210,7 +1195,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
@@ -1230,7 +1215,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
@@ -1250,7 +1235,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
@@ -1269,11 +1254,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>17</v>
+      <c r="A10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
@@ -1293,7 +1278,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -1313,7 +1298,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
@@ -1333,7 +1318,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
@@ -1352,170 +1337,36 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D14">
-        <v>1.0</v>
-      </c>
-      <c r="E14">
-        <v>1.0</v>
-      </c>
-      <c r="F14">
-        <v>1.0</v>
-      </c>
-      <c r="G14">
-        <v>1.0</v>
-      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D15">
-        <v>1.0</v>
-      </c>
-      <c r="E15">
-        <v>1.0</v>
-      </c>
-      <c r="F15">
-        <v>1.0</v>
-      </c>
-      <c r="G15">
-        <v>1.0</v>
-      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D16">
-        <v>1.0</v>
-      </c>
-      <c r="E16">
-        <v>1.0</v>
-      </c>
-      <c r="F16">
-        <v>1.0</v>
-      </c>
-      <c r="G16">
-        <v>1.0</v>
-      </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D17">
-        <v>1.0</v>
-      </c>
-      <c r="E17">
-        <v>1.0</v>
-      </c>
-      <c r="F17">
-        <v>1.0</v>
-      </c>
-      <c r="G17">
-        <v>1.0</v>
-      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D18">
-        <v>1.0</v>
-      </c>
-      <c r="E18">
-        <v>1.0</v>
-      </c>
-      <c r="F18">
-        <v>1.0</v>
-      </c>
-      <c r="G18">
-        <v>1.0</v>
-      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19">
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D19">
-        <v>1.0</v>
-      </c>
-      <c r="E19">
-        <v>1.0</v>
-      </c>
-      <c r="F19">
-        <v>1.0</v>
-      </c>
-      <c r="G19">
-        <v>1.0</v>
-      </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21">
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1.0</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1534,7 +1385,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1557,7 +1408,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -1577,7 +1428,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
@@ -1597,7 +1448,7 @@
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -1617,7 +1468,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -1640,7 +1491,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
@@ -1660,7 +1511,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
@@ -1680,7 +1531,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
@@ -1700,7 +1551,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
@@ -1723,7 +1574,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
@@ -1743,7 +1594,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -1763,7 +1614,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
@@ -1783,7 +1634,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
@@ -1806,7 +1657,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
@@ -1826,7 +1677,7 @@
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
@@ -1846,7 +1697,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
@@ -1866,7 +1717,7 @@
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
@@ -1889,7 +1740,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -1909,7 +1760,7 @@
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
@@ -1929,7 +1780,7 @@
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
@@ -1949,7 +1800,7 @@
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
@@ -1973,6 +1824,456 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D2">
+        <v>1.0</v>
+      </c>
+      <c r="E2">
+        <v>1.0</v>
+      </c>
+      <c r="F2">
+        <v>1.0</v>
+      </c>
+      <c r="G2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D6">
+        <v>1.0</v>
+      </c>
+      <c r="E6">
+        <v>1.0</v>
+      </c>
+      <c r="F6">
+        <v>1.0</v>
+      </c>
+      <c r="G6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D10">
+        <v>1.0</v>
+      </c>
+      <c r="E10">
+        <v>1.0</v>
+      </c>
+      <c r="F10">
+        <v>1.0</v>
+      </c>
+      <c r="G10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D11">
+        <v>1.0</v>
+      </c>
+      <c r="E11">
+        <v>1.0</v>
+      </c>
+      <c r="F11">
+        <v>1.0</v>
+      </c>
+      <c r="G11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D14">
+        <v>1.0</v>
+      </c>
+      <c r="E14">
+        <v>1.0</v>
+      </c>
+      <c r="F14">
+        <v>1.0</v>
+      </c>
+      <c r="G14">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D15">
+        <v>1.0</v>
+      </c>
+      <c r="E15">
+        <v>1.0</v>
+      </c>
+      <c r="F15">
+        <v>1.0</v>
+      </c>
+      <c r="G15">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D16">
+        <v>1.0</v>
+      </c>
+      <c r="E16">
+        <v>1.0</v>
+      </c>
+      <c r="F16">
+        <v>1.0</v>
+      </c>
+      <c r="G16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D17">
+        <v>1.0</v>
+      </c>
+      <c r="E17">
+        <v>1.0</v>
+      </c>
+      <c r="F17">
+        <v>1.0</v>
+      </c>
+      <c r="G17">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D18">
+        <v>1.0</v>
+      </c>
+      <c r="E18">
+        <v>1.0</v>
+      </c>
+      <c r="F18">
+        <v>1.0</v>
+      </c>
+      <c r="G18">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D19">
+        <v>1.0</v>
+      </c>
+      <c r="E19">
+        <v>1.0</v>
+      </c>
+      <c r="F19">
+        <v>1.0</v>
+      </c>
+      <c r="G19">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1987,7 +2288,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -2010,7 +2311,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -2030,7 +2331,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
@@ -2050,7 +2351,7 @@
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -2070,7 +2371,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -2093,7 +2394,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
@@ -2113,7 +2414,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
@@ -2133,7 +2434,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
@@ -2153,7 +2454,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
@@ -2176,7 +2477,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
@@ -2196,7 +2497,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -2216,7 +2517,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
@@ -2236,7 +2537,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
@@ -2259,7 +2560,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
@@ -2279,7 +2580,7 @@
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
@@ -2299,7 +2600,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
@@ -2319,7 +2620,7 @@
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
@@ -2342,7 +2643,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -2362,7 +2663,7 @@
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
@@ -2382,7 +2683,7 @@
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
@@ -2402,7 +2703,7 @@
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
@@ -2425,7 +2726,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2">
         <v>1.0</v>
@@ -2445,7 +2746,7 @@
     </row>
     <row r="23">
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2">
         <v>1.0</v>
@@ -2465,7 +2766,7 @@
     </row>
     <row r="24">
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" s="2">
         <v>1.0</v>
@@ -2485,7 +2786,7 @@
     </row>
     <row r="25">
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2">
         <v>1.0</v>
@@ -2508,7 +2809,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
@@ -2528,7 +2829,7 @@
     </row>
     <row r="27">
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
@@ -2548,7 +2849,7 @@
     </row>
     <row r="28">
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
@@ -2568,7 +2869,7 @@
     </row>
     <row r="29">
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
@@ -2637,322 +2938,6 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D2">
-        <v>1.0</v>
-      </c>
-      <c r="E2">
-        <v>1.0</v>
-      </c>
-      <c r="F2">
-        <v>1.0</v>
-      </c>
-      <c r="G2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D6">
-        <v>1.0</v>
-      </c>
-      <c r="E6">
-        <v>1.0</v>
-      </c>
-      <c r="F6">
-        <v>1.0</v>
-      </c>
-      <c r="G6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D10">
-        <v>1.0</v>
-      </c>
-      <c r="E10">
-        <v>1.0</v>
-      </c>
-      <c r="F10">
-        <v>1.0</v>
-      </c>
-      <c r="G10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D11">
-        <v>1.0</v>
-      </c>
-      <c r="E11">
-        <v>1.0</v>
-      </c>
-      <c r="F11">
-        <v>1.0</v>
-      </c>
-      <c r="G11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19">
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2967,60 +2952,31 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="2"/>
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>43</v>
+      <c r="A2" s="2">
+        <v>2.0</v>
       </c>
       <c r="B2" s="2">
-        <v>0.0543</v>
+        <v>2.0</v>
       </c>
       <c r="C2" s="2">
-        <v>0.1711</v>
+        <v>2.0</v>
       </c>
       <c r="D2" s="2">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.1048</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -3037,30 +2993,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>0.2258</v>
-      </c>
       <c r="B2" s="2">
-        <v>0.0705</v>
+        <v>0.0543</v>
       </c>
       <c r="C2" s="2">
-        <v>0.134</v>
+        <v>0.1711</v>
       </c>
       <c r="D2" s="2">
-        <v>0.5698</v>
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.1048</v>
       </c>
     </row>
   </sheetData>
@@ -3077,24 +3062,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>0.0198</v>
+        <v>0.2258</v>
       </c>
       <c r="B2" s="2">
-        <v>0.1032</v>
+        <v>0.0705</v>
       </c>
       <c r="C2" s="2">
-        <v>0.7419</v>
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.5698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduce mortality to below 1000
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -258,10 +258,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -377,19 +377,19 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>1000.0</v>
+        <v>500.0</v>
       </c>
       <c r="B2" s="1">
-        <v>1000.0</v>
+        <v>500.0</v>
       </c>
       <c r="C2" s="1">
-        <v>1000.0</v>
+        <v>500.0</v>
       </c>
       <c r="D2" s="1">
-        <v>1000.0</v>
+        <v>500.0</v>
       </c>
       <c r="E2" s="1">
-        <v>1000.0</v>
+        <v>500.0</v>
       </c>
     </row>
   </sheetData>
@@ -452,59 +452,59 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>0.0543</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.1711</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>3.0E-4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>0.009</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0.3607</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>0.0085</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
         <v>0.2908</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>0.1048</v>
       </c>
     </row>
@@ -521,30 +521,30 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>0.2258</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>0.0705</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.134</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>0.5698</v>
       </c>
     </row>
@@ -561,7 +561,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -572,13 +572,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>0.0198</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>0.1032</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.7419</v>
       </c>
     </row>
@@ -595,66 +595,66 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>3.14</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>1.73</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>1.73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>1.6</v>
       </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
         <v>1.57</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>1.6</v>
       </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
         <v>1.57</v>
       </c>
     </row>
@@ -662,44 +662,44 @@
       <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>1.75</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>1.75</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>1.75</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1.4</v>
       </c>
-      <c r="D6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
         <v>1.33</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>1.4</v>
       </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
         <v>1.33</v>
       </c>
     </row>
@@ -707,44 +707,44 @@
       <c r="A8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>1.52</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>1.52</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>1.52</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>1.2</v>
       </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1.2</v>
       </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -761,36 +761,36 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="3">
         <v>3.03</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>1.77</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -798,16 +798,16 @@
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
         <v>1.49</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>1.1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -815,16 +815,16 @@
       <c r="A4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
         <v>1.41</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>1.18</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -905,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="2">
         <v>0.0</v>
@@ -1064,27 +1064,27 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.0</v>
       </c>
       <c r="C10" s="2">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="D10" s="2">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="E10" s="2">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="F10" s="2">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0.0</v>
       </c>
       <c r="C11" s="2">
@@ -1104,7 +1104,7 @@
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0.0</v>
       </c>
       <c r="C12" s="2">
@@ -1227,16 +1227,16 @@
       <c r="B18" s="2">
         <v>0.0</v>
       </c>
-      <c r="C18" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="C18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="2">
         <v>0.0</v>
       </c>
     </row>
@@ -1253,10 +1253,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C1" t="s">
@@ -1276,13 +1276,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2">
@@ -1299,73 +1299,73 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1.0</v>
       </c>
       <c r="D6">
@@ -1382,73 +1382,73 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1.0</v>
       </c>
       <c r="D10">
@@ -1465,10 +1465,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>1.0</v>
       </c>
       <c r="D11">
@@ -1485,76 +1485,76 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="2"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15">
-      <c r="C15" s="2"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16">
-      <c r="C16" s="2"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17">
-      <c r="C17" s="2"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18">
-      <c r="C18" s="2"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19">
-      <c r="C19" s="2"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1569,10 +1569,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C1" t="s">
@@ -1595,10 +1595,10 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2">
@@ -1615,62 +1615,62 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -1678,10 +1678,10 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1.0</v>
       </c>
       <c r="D6">
@@ -1698,62 +1698,62 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -1761,10 +1761,10 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1.0</v>
       </c>
       <c r="D10">
@@ -1781,10 +1781,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>1.0</v>
       </c>
       <c r="D11">
@@ -1801,42 +1801,42 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -1844,10 +1844,10 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>1.0</v>
       </c>
       <c r="D14">
@@ -1864,10 +1864,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>1.0</v>
       </c>
       <c r="D15">
@@ -1884,10 +1884,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>1.0</v>
       </c>
       <c r="D16">
@@ -1904,10 +1904,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>1.0</v>
       </c>
       <c r="D17">
@@ -1927,10 +1927,10 @@
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>1.0</v>
       </c>
       <c r="D18">
@@ -1947,10 +1947,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>1.0</v>
       </c>
       <c r="D19">
@@ -1967,42 +1967,42 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="C20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="C21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G21" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2019,10 +2019,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C1" t="s">
@@ -2045,10 +2045,10 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2">
@@ -2065,62 +2065,62 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2128,10 +2128,10 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1.0</v>
       </c>
       <c r="D6">
@@ -2148,62 +2148,62 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2211,10 +2211,10 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1.0</v>
       </c>
       <c r="D10">
@@ -2231,10 +2231,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>1.0</v>
       </c>
       <c r="D11">
@@ -2251,42 +2251,42 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2294,10 +2294,10 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>1.0</v>
       </c>
       <c r="D14">
@@ -2314,10 +2314,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>1.0</v>
       </c>
       <c r="D15">
@@ -2334,10 +2334,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>1.0</v>
       </c>
       <c r="D16">
@@ -2354,10 +2354,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>1.0</v>
       </c>
       <c r="D17">
@@ -2377,10 +2377,10 @@
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>1.0</v>
       </c>
       <c r="D18">
@@ -2397,10 +2397,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>1.0</v>
       </c>
       <c r="D19">
@@ -2417,42 +2417,42 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="C20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="C21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G21" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2472,10 +2472,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C1" t="s">
@@ -2498,10 +2498,10 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2">
@@ -2518,62 +2518,62 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2581,10 +2581,10 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1.0</v>
       </c>
       <c r="D6">
@@ -2601,62 +2601,62 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2664,10 +2664,10 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1.0</v>
       </c>
       <c r="D10">
@@ -2684,10 +2684,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>1.0</v>
       </c>
       <c r="D11">
@@ -2704,42 +2704,42 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2747,10 +2747,10 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>1.0</v>
       </c>
       <c r="D14">
@@ -2767,10 +2767,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>1.0</v>
       </c>
       <c r="D15">
@@ -2787,10 +2787,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>1.0</v>
       </c>
       <c r="D16">
@@ -2807,10 +2807,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>1.0</v>
       </c>
       <c r="D17">
@@ -2830,10 +2830,10 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>1.0</v>
       </c>
       <c r="D18">
@@ -2850,10 +2850,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>1.0</v>
       </c>
       <c r="D19">
@@ -2870,42 +2870,42 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="C20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="C21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G21" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2913,10 +2913,10 @@
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>1.0</v>
       </c>
       <c r="D22">
@@ -2933,62 +2933,62 @@
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="C23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G23" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G24" s="2">
+      <c r="C24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G24" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="C25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G25" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -2996,10 +2996,10 @@
       <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>1.0</v>
       </c>
       <c r="D26">
@@ -3016,116 +3016,116 @@
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G27" s="2">
+      <c r="C27" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G27" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G28" s="2">
+      <c r="C28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G28" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G29" s="2">
+      <c r="C29" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G29" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="2"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31">
-      <c r="C31" s="2"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34">
-      <c r="C34" s="2"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35">
-      <c r="C35" s="2"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36">
-      <c r="C36" s="2"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37">
-      <c r="C37" s="2"/>
+      <c r="C37" s="3"/>
     </row>
     <row r="38">
-      <c r="C38" s="2"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39">
-      <c r="C39" s="2"/>
+      <c r="C39" s="3"/>
     </row>
     <row r="40">
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3154,16 +3154,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>2.0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>2.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>2.0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix distributions to be normalised
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -255,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -268,6 +268,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -423,102 +427,102 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="B2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>2.0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="9">
         <v>2.0</v>
       </c>
-      <c r="D3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="D3" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>2.0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="9">
         <v>2.0</v>
       </c>
-      <c r="D4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="D4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <v>2.0</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="9">
         <v>2.0</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="9">
         <v>2.0</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="9">
         <v>2.0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="8">
         <v>1.0</v>
       </c>
     </row>
@@ -693,10 +697,10 @@
       <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -788,7 +792,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -833,7 +837,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -924,7 +928,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="3">
@@ -941,7 +945,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="3">
@@ -970,21 +974,21 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="12">
         <v>1.0</v>
       </c>
       <c r="B2" s="1">
@@ -1411,80 +1415,80 @@
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D2">
-        <v>1.0</v>
-      </c>
-      <c r="E2">
-        <v>1.0</v>
-      </c>
-      <c r="F2">
-        <v>1.0</v>
-      </c>
-      <c r="G2">
-        <v>1.0</v>
+      <c r="C2" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1.0</v>
+      <c r="C3" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1.0</v>
+      <c r="C4" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.0</v>
+      <c r="C5" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="6">
@@ -1494,80 +1498,80 @@
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D6">
-        <v>1.0</v>
-      </c>
-      <c r="E6">
-        <v>1.0</v>
-      </c>
-      <c r="F6">
-        <v>1.0</v>
-      </c>
-      <c r="G6">
-        <v>1.0</v>
+      <c r="C6" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1.0</v>
+      <c r="C7" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1.0</v>
+      <c r="C8" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1.0</v>
+      <c r="C9" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="10">
@@ -1577,84 +1581,84 @@
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10">
-        <v>1.0</v>
-      </c>
-      <c r="E10">
-        <v>1.0</v>
-      </c>
-      <c r="F10">
-        <v>1.0</v>
-      </c>
-      <c r="G10">
-        <v>1.0</v>
+      <c r="C10" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D11">
-        <v>1.0</v>
-      </c>
-      <c r="E11">
-        <v>1.0</v>
-      </c>
-      <c r="F11">
-        <v>1.0</v>
-      </c>
-      <c r="G11">
-        <v>1.0</v>
+      <c r="C11" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1.0</v>
+      <c r="C12" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1.0</v>
+      <c r="C13" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>25.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="3"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15">
       <c r="C15" s="3"/>
@@ -3273,155 +3277,155 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="B2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="B3" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="9">
         <v>10.0</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="9">
         <v>10.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="B4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="9">
         <v>10.0</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="9">
         <v>10.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="B5" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="9">
         <v>10.0</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="9">
         <v>10.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="9">
         <v>100.0</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="9">
         <v>100.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="B7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="B8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="B9" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="8">
         <v>1.0</v>
       </c>
     </row>
@@ -3478,36 +3482,36 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8">
+      <c r="A2" s="10">
         <v>0.3</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="10">
         <v>0.3</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="10">
         <v>0.3</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="10">
         <v>0.3</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="10">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rename tabs, generalise by intervention and condition
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -11,16 +11,16 @@
     <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="RR Death by Birth Outcome" sheetId="7" r:id="rId9"/>
     <sheet state="visible" name="OR stunting progression" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="Incidence diarrhoea" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="Incidence of conditions" sheetId="9" r:id="rId11"/>
     <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="OR stunting diarrhoea" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="OR stunting Zinc" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="birth distribution" sheetId="13" r:id="rId15"/>
     <sheet state="visible" name="time between births" sheetId="14" r:id="rId16"/>
     <sheet state="visible" name="birth outcome distribution" sheetId="15" r:id="rId17"/>
     <sheet state="visible" name="RR birth by type" sheetId="16" r:id="rId18"/>
     <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="OR birth outcome stunting" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="18" r:id="rId20"/>
     <sheet state="visible" name="Interventions coverages" sheetId="19" r:id="rId21"/>
     <sheet state="visible" name="Interventions affected fraction" sheetId="20" r:id="rId22"/>
     <sheet state="visible" name="Interventions mortality eff" sheetId="21" r:id="rId23"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="69">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -182,9 +182,18 @@
     <t>Neonatal congenital anomalies</t>
   </si>
   <si>
+    <t>Condition</t>
+  </si>
+  <si>
     <t>Breastfeeding Category</t>
   </si>
   <si>
+    <t>Intervention</t>
+  </si>
+  <si>
+    <t>Zinc supplementation</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -218,13 +227,7 @@
     <t>Outcome</t>
   </si>
   <si>
-    <t>Intervention</t>
-  </si>
-  <si>
     <t>pre-2016</t>
-  </si>
-  <si>
-    <t>Zinc supplementation</t>
   </si>
   <si>
     <t>Vitamin A supplementation</t>
@@ -495,7 +498,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -606,25 +609,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1.04</v>
+      <c r="A2" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1.04</v>
@@ -636,6 +642,9 @@
         <v>1.04</v>
       </c>
       <c r="E2">
+        <v>1.04</v>
+      </c>
+      <c r="F2">
         <v>1.04</v>
       </c>
     </row>
@@ -652,25 +661,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
-        <v>0.9</v>
+      <c r="A2" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="3">
         <v>0.9</v>
@@ -682,6 +694,9 @@
         <v>0.9</v>
       </c>
       <c r="E2" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="3">
         <v>0.9</v>
       </c>
     </row>
@@ -699,22 +714,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3">
         <v>0.0</v>
@@ -728,7 +743,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3">
         <v>0.0</v>
@@ -742,7 +757,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -768,16 +783,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -842,19 +857,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -862,7 +877,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3">
         <v>3.0</v>
@@ -877,7 +892,7 @@
     <row r="3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3">
         <v>1.0</v>
@@ -892,7 +907,7 @@
     <row r="4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3">
         <v>1.0</v>
@@ -909,7 +924,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3">
         <v>2.0</v>
@@ -923,7 +938,7 @@
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3">
         <v>1.0</v>
@@ -937,7 +952,7 @@
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3">
         <v>1.0</v>
@@ -954,7 +969,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3">
         <v>2.0</v>
@@ -968,7 +983,7 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C9" s="3">
         <v>1.0</v>
@@ -982,7 +997,7 @@
     </row>
     <row r="10">
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3">
         <v>1.0</v>
@@ -1008,19 +1023,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -1132,16 +1147,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3">
         <v>0.0</v>
@@ -1154,7 +1169,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3">
         <v>0.0</v>
@@ -1166,7 +1181,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -1178,7 +1193,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3">
         <v>0.0</v>
@@ -1190,7 +1205,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3">
         <v>0.0</v>
@@ -1202,7 +1217,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3">
         <v>0.0</v>
@@ -1214,7 +1229,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3">
         <v>0.0</v>
@@ -1226,7 +1241,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3">
         <v>0.0</v>
@@ -1238,7 +1253,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3">
         <v>0.0</v>
@@ -1731,7 +1746,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -1754,7 +1769,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
@@ -1798,7 +1813,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -1874,7 +1889,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -1897,7 +1912,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
@@ -1941,7 +1956,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -2017,7 +2032,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2040,7 +2055,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
@@ -2084,7 +2099,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -4256,24 +4271,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
-        <v>0.3</v>
+      <c r="A2" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="10">
         <v>0.3</v>
@@ -4285,7 +4303,30 @@
         <v>0.3</v>
       </c>
       <c r="E2" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="10">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified constatnts.py to generalise quartic evaluation so that we use it for complementary feeding as well as birth outcomes.  Now calculating complementary feeding probabilities.  Added complementary feeding reading from spreadsheet to data.py.
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -15,17 +15,18 @@
     <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
     <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
     <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
-    <sheet state="visible" name="birth distribution" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="time between births" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="RR birth by type" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="OR stunting by birth outcome" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions maternal" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="22" r:id="rId24"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="OR stunting for complements" sheetId="13" r:id="rId15"/>
+    <sheet state="visible" name="birth distribution" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="time between births" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="RR birth by type" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="RR birth by time" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="24" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="76">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -193,6 +194,21 @@
   </si>
   <si>
     <t>Zinc supplementation</t>
+  </si>
+  <si>
+    <t>Complements group</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food secure with promotion)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food secure without promotion)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with promotion and supplementation)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
   </si>
   <si>
     <t>Type</t>
@@ -423,6 +439,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -723,62 +743,108 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="70.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="3">
-        <v>0.2</v>
+        <v>1.0</v>
       </c>
       <c r="D2" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" s="3">
-        <v>0.4</v>
+        <v>1.0</v>
       </c>
       <c r="D3" s="3">
-        <v>0.0</v>
+        <v>1.43</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.43</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" s="3">
-        <v>0.3</v>
+        <v>1.0</v>
       </c>
       <c r="D4" s="3">
-        <v>0.1</v>
+        <v>1.6</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.39</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.39</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -795,30 +861,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
+      <c r="B2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="3">
         <v>0.2</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
       <c r="D2" s="3">
-        <v>0.6</v>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -835,24 +930,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>40</v>
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="B2" s="3">
         <v>0.0</v>
       </c>
       <c r="C2" s="3">
-        <v>0.7</v>
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -869,156 +970,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>52</v>
+      <c r="A2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -1035,25 +1004,191 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B2" s="3">
         <v>1.0</v>
       </c>
@@ -1106,7 +1241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1146,7 +1281,379 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1162,7 +1669,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -1181,7 +1688,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3">
         <v>0.0</v>
@@ -1193,7 +1700,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -1205,7 +1712,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3">
         <v>0.0</v>
@@ -1217,7 +1724,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3">
         <v>0.0</v>
@@ -1229,7 +1736,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3">
         <v>0.0</v>
@@ -1241,7 +1748,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3">
         <v>0.0</v>
@@ -1253,7 +1760,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3">
         <v>0.0</v>
@@ -1265,7 +1772,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B10" s="3">
         <v>0.0</v>
@@ -1377,379 +1884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1761,7 +1896,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -1778,10 +1913,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C2" s="13">
         <v>0.35</v>
@@ -1798,7 +1933,7 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C3" s="13">
         <v>0.0</v>
@@ -1815,10 +1950,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" s="13">
         <v>0.31</v>
@@ -1835,7 +1970,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C5" s="13">
         <v>0.336</v>
@@ -1852,10 +1987,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C6" s="13">
         <v>0.09</v>
@@ -1872,7 +2007,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C7" s="13">
         <v>1.0</v>
@@ -1886,149 +2021,6 @@
       <c r="F7" s="13">
         <v>0.0</v>
       </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.416</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0.416</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.416</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2044,7 +2036,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2081,11 +2073,11 @@
       <c r="E2" s="3">
         <v>0.0</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.5</v>
+      <c r="F2" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.253</v>
       </c>
     </row>
     <row r="3">
@@ -2102,16 +2094,16 @@
       <c r="E3" s="3">
         <v>0.0</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.51</v>
+      <c r="F3" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -2123,13 +2115,13 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.3</v>
+        <v>0.416</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.416</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.416</v>
       </c>
     </row>
     <row r="5">
@@ -2187,7 +2179,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2225,10 +2217,10 @@
         <v>0.0</v>
       </c>
       <c r="F2" s="3">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="G2" s="3">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -2246,6 +2238,149 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.52</v>
       </c>
       <c r="G3" s="3">
@@ -2254,7 +2389,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
added new tabs to testing spreaddheet so that the tests run
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -16,17 +16,18 @@
     <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
     <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="OR stunting for complements" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="birth distribution" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="time between births" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="RR birth by type" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="RR birth by time" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="OR stunting by birth outcome" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="Interventions maternal" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="22" r:id="rId24"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="23" r:id="rId25"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="24" r:id="rId26"/>
+    <sheet state="visible" name="OR exclusiveBF by intervention" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="birth distribution" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="time between births" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="RR birth by type" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="RR birth by time" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="24" r:id="rId26"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="25" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="77">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -209,6 +210,9 @@
   </si>
   <si>
     <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
+  </si>
+  <si>
+    <t>Breastfeeding promotion - Health system &amp; Home/community</t>
   </si>
   <si>
     <t>Type</t>
@@ -287,7 +291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -301,6 +305,9 @@
     <font/>
     <font>
       <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -355,6 +362,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -443,6 +456,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -858,63 +875,69 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="37.29"/>
+    <col customWidth="1" min="2" max="2" width="10.71"/>
+    <col customWidth="1" min="3" max="3" width="12.71"/>
+    <col customWidth="1" min="4" max="4" width="11.14"/>
+    <col customWidth="1" min="5" max="6" width="12.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
+        <v>53</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2.3</v>
+      </c>
+      <c r="C2" s="11">
+        <v>4.6</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1.57</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -930,30 +953,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.6</v>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -970,24 +1022,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>40</v>
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="B2" s="3">
         <v>0.0</v>
       </c>
       <c r="C2" s="3">
-        <v>0.7</v>
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -1004,156 +1062,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>57</v>
+      <c r="A2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -1170,27 +1096,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="3">
-        <v>1.0</v>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="3">
         <v>3.0</v>
@@ -1199,40 +1125,126 @@
         <v>2.0</v>
       </c>
       <c r="E2" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -1249,31 +1261,71 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5.0</v>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1654,6 +1706,46 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1669,7 +1761,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -1688,7 +1780,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3">
         <v>0.0</v>
@@ -1700,7 +1792,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -1712,7 +1804,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3">
         <v>0.0</v>
@@ -1724,7 +1816,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3">
         <v>0.0</v>
@@ -1736,7 +1828,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3">
         <v>0.0</v>
@@ -1748,7 +1840,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3">
         <v>0.0</v>
@@ -1760,7 +1852,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3">
         <v>0.0</v>
@@ -1772,7 +1864,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3">
         <v>0.0</v>
@@ -1884,7 +1976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1896,7 +1988,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -1913,257 +2005,114 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="13">
+        <v>74</v>
+      </c>
+      <c r="C2" s="15">
         <v>0.35</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="15">
         <v>0.35</v>
       </c>
-      <c r="E2" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="15">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="13">
+        <v>75</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="15">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="13">
+        <v>74</v>
+      </c>
+      <c r="C4" s="15">
         <v>0.31</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="15">
         <v>0.31</v>
       </c>
-      <c r="E4" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="15">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="13">
+        <v>75</v>
+      </c>
+      <c r="C5" s="15">
         <v>0.336</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="15">
         <v>0.336</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="15">
         <v>0.336</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="15">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="13">
+        <v>74</v>
+      </c>
+      <c r="C6" s="15">
         <v>0.09</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="15">
         <v>0.09</v>
       </c>
-      <c r="E6" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="15">
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.416</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0.416</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.416</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C7" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2179,7 +2128,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2216,11 +2165,11 @@
       <c r="E2" s="3">
         <v>0.0</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.5</v>
+      <c r="F2" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.253</v>
       </c>
     </row>
     <row r="3">
@@ -2237,16 +2186,16 @@
       <c r="E3" s="3">
         <v>0.0</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.51</v>
+      <c r="F3" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -2258,23 +2207,23 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.3</v>
+        <v>0.416</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.416</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.416</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="17">
         <v>0.0</v>
       </c>
       <c r="E5" s="8">
@@ -2322,7 +2271,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2360,10 +2309,10 @@
         <v>0.0</v>
       </c>
       <c r="F2" s="3">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="G2" s="3">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -2381,6 +2330,149 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.52</v>
       </c>
       <c r="G3" s="3">
@@ -2389,7 +2481,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -2411,13 +2503,13 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="17">
         <v>0.0</v>
       </c>
       <c r="E5" s="8">

</xml_diff>

<commit_message>
updated test spreadsheet so that tests run
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -16,18 +16,19 @@
     <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
     <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="OR stunting for complements" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="OR exclusiveBF by intervention" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="birth distribution" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="time between births" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="RR birth by type" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="RR birth by time" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="OR stunting by birth outcome" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="Interventions maternal" sheetId="22" r:id="rId24"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="23" r:id="rId25"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="24" r:id="rId26"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="25" r:id="rId27"/>
+    <sheet state="visible" name="OR appropriateBF by interventio" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="Appropriate breastfeeding" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="birth distribution" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="time between births" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="RR birth by type" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="RR birth by time" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="24" r:id="rId26"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="25" r:id="rId27"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="26" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="76">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -215,6 +216,30 @@
     <t>Breastfeeding promotion - Health system &amp; Home/community</t>
   </si>
   <si>
+    <t>baseline coverage</t>
+  </si>
+  <si>
+    <t>saturation coverage</t>
+  </si>
+  <si>
+    <t>unit cost</t>
+  </si>
+  <si>
+    <t>Vitamin A supplementation</t>
+  </si>
+  <si>
+    <t>Complementary feeding</t>
+  </si>
+  <si>
+    <t>IPTp</t>
+  </si>
+  <si>
+    <t>Balanced energy supplementation</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -246,33 +271,6 @@
   </si>
   <si>
     <t>Outcome</t>
-  </si>
-  <si>
-    <t>pre-2016</t>
-  </si>
-  <si>
-    <t>Vitamin A supplementation</t>
-  </si>
-  <si>
-    <t>Complementary feeding 1</t>
-  </si>
-  <si>
-    <t>Complementary feeding 2</t>
-  </si>
-  <si>
-    <t>Complementary feeding 3</t>
-  </si>
-  <si>
-    <t>Breastfeeding promotion</t>
-  </si>
-  <si>
-    <t>IPTp</t>
-  </si>
-  <si>
-    <t>Balanced energy supplementation</t>
-  </si>
-  <si>
-    <t>Multiple micronutrient supplementation</t>
   </si>
   <si>
     <t>effectiveness</t>
@@ -329,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -367,6 +365,18 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -374,12 +384,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -457,6 +461,10 @@
 </file>
 
 <file path=xl/drawings/worksheetdrawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing26.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -950,63 +958,57 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="5" width="13.43"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1014,738 +1016,6 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1757,118 +1027,147 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="3"/>
+      <c r="B1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.85</v>
+      </c>
+      <c r="D2" s="16">
+        <v>60.0</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="5"/>
+      <c r="A3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.19</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="D3" s="16">
+        <v>300.0</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="5"/>
+      <c r="A4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.385</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="16">
+        <v>300.0</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="A5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.296</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="D5" s="16">
+        <v>100.0</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="5"/>
+      <c r="A6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0.257</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="D6" s="16">
+        <v>20.0</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="5"/>
+      <c r="A7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="16">
+        <v>80.0</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="5"/>
+      <c r="A8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="16">
+        <v>90.0</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.0</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.0</v>
-      </c>
+      <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1976,7 +1275,808 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1988,7 +2088,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -2005,257 +2105,114 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="15">
+        <v>73</v>
+      </c>
+      <c r="C2" s="19">
         <v>0.35</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="19">
         <v>0.35</v>
       </c>
-      <c r="E2" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="E2" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="15">
+        <v>74</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="15">
+        <v>73</v>
+      </c>
+      <c r="C4" s="19">
         <v>0.31</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="19">
         <v>0.31</v>
       </c>
-      <c r="E4" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="E4" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="15">
+        <v>74</v>
+      </c>
+      <c r="C5" s="19">
         <v>0.336</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="19">
         <v>0.336</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="19">
         <v>0.336</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="15">
+      <c r="C6" s="19">
         <v>0.09</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="19">
         <v>0.09</v>
       </c>
-      <c r="E6" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="E6" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="15">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.253</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.416</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0.416</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.416</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2271,7 +2228,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2308,11 +2265,11 @@
       <c r="E2" s="3">
         <v>0.0</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.5</v>
+      <c r="F2" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.253</v>
       </c>
     </row>
     <row r="3">
@@ -2329,16 +2286,16 @@
       <c r="E3" s="3">
         <v>0.0</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.51</v>
+      <c r="F3" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -2350,23 +2307,23 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.3</v>
+        <v>0.416</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.416</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.416</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="C5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="16">
         <v>0.0</v>
       </c>
       <c r="E5" s="8">
@@ -2414,7 +2371,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2452,10 +2409,10 @@
         <v>0.0</v>
       </c>
       <c r="F2" s="3">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="G2" s="3">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -2473,6 +2430,149 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.52</v>
       </c>
       <c r="G3" s="3">
@@ -2481,7 +2581,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -2503,13 +2603,13 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="C5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="16">
         <v>0.0</v>
       </c>
       <c r="E5" s="8">

</xml_diff>

<commit_message>
updated test spreadsheet for tests to pass
</commit_message>
<xml_diff>
--- a/InputForCode_tests.xlsx
+++ b/InputForCode_tests.xlsx
@@ -232,6 +232,9 @@
     <t>Complementary feeding</t>
   </si>
   <si>
+    <t>Breastfeeding promotion (dual delivery)</t>
+  </si>
+  <si>
     <t>IPTp</t>
   </si>
   <si>
@@ -242,9 +245,6 @@
   </si>
   <si>
     <t>pregnant women</t>
-  </si>
-  <si>
-    <t>Breastfeeding promotion (dual delivery)</t>
   </si>
   <si>
     <t>Outcome</t>
@@ -1218,8 +1218,8 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="16" t="s">
-        <v>53</v>
+      <c r="A5" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B5" s="18">
         <v>0.296</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="18">
         <v>0.257</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="18">
         <v>0.0</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="18">
         <v>0.0</v>
@@ -1433,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -1507,7 +1507,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B5" s="19">
         <v>1.0</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="19">
         <v>0.0</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="19">
         <v>0.0</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="19">
         <v>0.0</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>

</xml_diff>